<commit_message>
allocation algorithm updated final final
</commit_message>
<xml_diff>
--- a/test/official_test_case_2.xlsx
+++ b/test/official_test_case_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/limnaroline/forecasting-project/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4BCA94D-96C6-D645-A8DA-4375C5D135DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB50AA4-A035-4F47-A7FE-09BFFC2EA7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17600" yWindow="1660" windowWidth="14940" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funding" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>Source ID</t>
   </si>
@@ -110,18 +110,12 @@
     <t>Salary</t>
   </si>
   <si>
-    <t>12/31/2025</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
     <t>Salary, Equipment</t>
   </si>
   <si>
-    <t>6/30/2025</t>
-  </si>
-  <si>
     <t>Travel</t>
   </si>
   <si>
@@ -201,27 +195,16 @@
   </si>
   <si>
     <t>E010</t>
-  </si>
-  <si>
-    <t>3/15/2025</t>
-  </si>
-  <si>
-    <t>5/20/2025</t>
-  </si>
-  <si>
-    <t>7/15/2025</t>
-  </si>
-  <si>
-    <t>8/20/2025</t>
-  </si>
-  <si>
-    <t>11/15/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="d/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,14 +234,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -559,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -593,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -601,10 +587,10 @@
       <c r="D2" s="1">
         <v>45658</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F2" s="2">
         <v>30000</v>
       </c>
     </row>
@@ -613,18 +599,18 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1">
         <v>45658</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F3" s="2">
         <v>25000</v>
       </c>
     </row>
@@ -633,18 +619,18 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1">
         <v>45658</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F4" s="2">
         <v>20000</v>
       </c>
     </row>
@@ -653,7 +639,7 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -661,10 +647,10 @@
       <c r="D5" s="1">
         <v>45658</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="5">
+        <v>45838</v>
+      </c>
+      <c r="F5" s="2">
         <v>10000</v>
       </c>
     </row>
@@ -673,18 +659,18 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1">
         <v>45658</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="5">
+        <v>45838</v>
+      </c>
+      <c r="F6" s="2">
         <v>8000</v>
       </c>
     </row>
@@ -693,18 +679,18 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1">
         <v>45658</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F7" s="2">
         <v>12000</v>
       </c>
     </row>
@@ -713,18 +699,18 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1">
         <v>45658</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F8" s="2">
         <v>5000</v>
       </c>
     </row>
@@ -733,18 +719,18 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1">
         <v>45658</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9" s="5">
+        <v>45838</v>
+      </c>
+      <c r="F9" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -753,18 +739,18 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1">
         <v>45658</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F10" s="2">
         <v>2000</v>
       </c>
     </row>
@@ -773,7 +759,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -781,10 +767,10 @@
       <c r="D11" s="1">
         <v>45658</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F11" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -793,18 +779,18 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1">
         <v>45658</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F12" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -813,7 +799,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -821,10 +807,10 @@
       <c r="D13" s="1">
         <v>45658</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="E13" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F13" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -833,18 +819,18 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1">
         <v>45658</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="E14" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F14" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -853,18 +839,18 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="1">
-        <v>45664</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="3">
+        <v>45839</v>
+      </c>
+      <c r="E15" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F15" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -873,18 +859,18 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1">
-        <v>45664</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="3">
+        <v>45839</v>
+      </c>
+      <c r="E16" s="3">
+        <v>46022</v>
+      </c>
+      <c r="F16" s="2">
         <v>3000</v>
       </c>
     </row>
@@ -898,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -932,16 +918,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="3">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2">
         <v>8000</v>
       </c>
       <c r="F2" s="4">
-        <v>45932</v>
+        <v>45698</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -949,16 +935,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="3">
+        <v>31</v>
+      </c>
+      <c r="E3" s="2">
         <v>7000</v>
       </c>
       <c r="F3" s="4">
-        <v>45934</v>
+        <v>45757</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -966,16 +952,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="3">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2">
         <v>6000</v>
       </c>
       <c r="F4" s="4">
-        <v>45936</v>
+        <v>45818</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -983,16 +969,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>10000</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>60</v>
+      <c r="F5" s="4">
+        <v>45731</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1000,16 +986,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2">
         <v>12000</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>61</v>
+      <c r="F6" s="4">
+        <v>45797</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1017,16 +1003,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>9000</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>62</v>
+      <c r="F7" s="4">
+        <v>45853</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1034,16 +1020,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2">
         <v>10000</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>63</v>
+      <c r="F8" s="4">
+        <v>45889</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1051,12 +1037,12 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>8000</v>
       </c>
       <c r="F9" s="4">
@@ -1068,16 +1054,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2">
         <v>7000</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>64</v>
+      <c r="F10" s="4">
+        <v>45976</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1085,16 +1071,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="3">
+        <v>31</v>
+      </c>
+      <c r="E11" s="2">
         <v>5000</v>
       </c>
       <c r="F11" s="4">
-        <v>45942</v>
+        <v>46001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>